<commit_message>
ExcelReader Added to the DataController
</commit_message>
<xml_diff>
--- a/Excel/ADMIN_APIDataFile.xlsx
+++ b/Excel/ADMIN_APIDataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\outsource.minura\API_Testing\api-automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9CDF9D-FE9D-4535-9BB7-DF04C53F2130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC4811B-1879-410A-85F3-2586A251E918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
 }</t>
   </si>
   <si>
-    <t>Unable to find TaxType with id 10</t>
-  </si>
-  <si>
     <t>{
   "countryId": 1,
   "endDate": "2022-10-14",
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>Please enter either Tax Percentage or Tax Rate</t>
+  </si>
+  <si>
+    <t>Unable to find TaxType with id 12</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -582,7 +582,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="146.1" customHeight="1">
@@ -596,7 +596,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="135">
@@ -607,10 +607,10 @@
         <v>500</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>